<commit_message>
second half gmail only completed
</commit_message>
<xml_diff>
--- a/SecondHalf/SecondHalf/PasswordManager.xlsx
+++ b/SecondHalf/SecondHalf/PasswordManager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laur\Desktop\RPA\proiect\RPA-PasswordManager\SecondHalf\SecondHalf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A9E34D-C8AC-4146-B687-4BC5E04A6B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D488339-18A9-42E4-9947-7A1373FFFE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2430" yWindow="1845" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15"/>

</xml_diff>